<commit_message>
The function-list of myTools.
Update.
</commit_message>
<xml_diff>
--- a/myTools-FunctionList.xlsx
+++ b/myTools-FunctionList.xlsx
@@ -48,10 +48,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>翻转字符串的第i位到第j位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>显示</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -101,6 +97,10 @@
   </si>
   <si>
     <t>int length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>翻转字符串的第i位到第j位，成功时返回true</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -281,67 +281,67 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -651,7 +651,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -663,185 +663,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="17" t="s">
+    <row r="3" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="20"/>
+      <c r="B3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="22" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="20"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="20"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="20"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="20"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="20"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="20"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="20"/>
+      <c r="B10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="21"/>
+      <c r="B11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="D11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="2"/>
+      <c r="A13" s="22"/>
     </row>
     <row r="14" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="2"/>
+      <c r="A14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="2"/>
+      <c r="A15" s="22"/>
     </row>
     <row r="16" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2"/>
+      <c r="A16" s="22"/>
     </row>
     <row r="17" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="2"/>
+      <c r="A17" s="22"/>
     </row>
     <row r="18" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2"/>
+      <c r="A18" s="22"/>
     </row>
     <row r="19" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2"/>
+      <c r="A19" s="22"/>
     </row>
     <row r="20" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2"/>
+      <c r="A20" s="22"/>
     </row>
     <row r="21" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2"/>
+      <c r="A21" s="22"/>
     </row>
     <row r="22" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="22" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="2"/>
+      <c r="A23" s="22"/>
     </row>
     <row r="24" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2"/>
+      <c r="A24" s="22"/>
     </row>
     <row r="25" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="2"/>
+      <c r="A25" s="22"/>
     </row>
     <row r="26" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2"/>
+      <c r="A26" s="22"/>
     </row>
     <row r="27" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="2"/>
+      <c r="A27" s="22"/>
     </row>
     <row r="28" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="2"/>
+      <c r="A28" s="22"/>
     </row>
     <row r="29" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="2"/>
+      <c r="A29" s="22"/>
     </row>
     <row r="30" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="2"/>
+      <c r="A30" s="22"/>
     </row>
     <row r="31" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="2"/>
+      <c r="A31" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>